<commit_message>
Converted all books to txt format, removed 1 book from corpus
</commit_message>
<xml_diff>
--- a/Book Documentation.xlsx
+++ b/Book Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinh\Desktop\College Stuff\Comp Ling Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1EB344-4292-4407-8B2A-775023C681CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A92CC8-3F25-4A27-8056-2637D0004BDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C94EF9E2-1198-47B8-9388-E321FADA7C2F}"/>
   </bookViews>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE2798D-75E9-44CF-8467-CB97DDF729A5}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,7 +1918,7 @@
         <v>125</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Updated the files that were converted wrong
</commit_message>
<xml_diff>
--- a/Book Documentation.xlsx
+++ b/Book Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinh\Desktop\College Stuff\Comp Ling Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A92CC8-3F25-4A27-8056-2637D0004BDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D725C2F9-AECC-4987-B72B-7ED79B02BB00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C94EF9E2-1198-47B8-9388-E321FADA7C2F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="129">
   <si>
     <t>Title</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Doctor Zhivago</t>
-  </si>
-  <si>
-    <t>The Merchant of Venice</t>
   </si>
   <si>
     <t>The Tempest</t>
@@ -788,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE2798D-75E9-44CF-8467-CB97DDF729A5}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -868,7 +865,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -885,7 +882,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -910,7 +907,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -938,7 +935,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
@@ -952,7 +949,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -1036,7 +1033,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -1092,7 +1089,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>6</v>
@@ -1134,10 +1131,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1148,7 +1145,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>6</v>
@@ -1159,7 +1156,7 @@
         <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -1173,35 +1170,35 @@
         <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
         <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -1215,38 +1212,38 @@
         <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>6</v>
@@ -1260,7 +1257,7 @@
         <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>6</v>
@@ -1271,21 +1268,21 @@
         <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
@@ -1296,10 +1293,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>6</v>
@@ -1327,7 +1324,7 @@
         <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
@@ -1347,12 +1344,12 @@
         <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -1369,7 +1366,7 @@
         <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>6</v>
@@ -1383,7 +1380,7 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
@@ -1394,10 +1391,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>6</v>
@@ -1408,10 +1405,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
         <v>66</v>
-      </c>
-      <c r="B43" t="s">
-        <v>50</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>6</v>
@@ -1425,7 +1422,7 @@
         <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>6</v>
@@ -1436,10 +1433,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>6</v>
@@ -1453,7 +1450,7 @@
         <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>6</v>
@@ -1464,10 +1461,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
@@ -1478,10 +1475,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>6</v>
@@ -1492,10 +1489,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>6</v>
@@ -1506,10 +1503,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>6</v>
@@ -1520,10 +1517,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>6</v>
@@ -1534,10 +1531,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>6</v>
@@ -1548,10 +1545,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>6</v>
@@ -1565,7 +1562,7 @@
         <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>6</v>
@@ -1579,7 +1576,7 @@
         <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>6</v>
@@ -1590,10 +1587,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
@@ -1604,10 +1601,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B57" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>6</v>
@@ -1618,10 +1615,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>6</v>
@@ -1632,10 +1629,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>6</v>
@@ -1646,10 +1643,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="s">
         <v>96</v>
-      </c>
-      <c r="B60" t="s">
-        <v>97</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>6</v>
@@ -1663,7 +1660,7 @@
         <v>98</v>
       </c>
       <c r="B61" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>6</v>
@@ -1674,10 +1671,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>6</v>
@@ -1688,10 +1685,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>6</v>
@@ -1702,10 +1699,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>6</v>
@@ -1716,10 +1713,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B65" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>6</v>
@@ -1730,10 +1727,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" t="s">
         <v>107</v>
-      </c>
-      <c r="B66" t="s">
-        <v>108</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>6</v>
@@ -1747,7 +1744,7 @@
         <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>6</v>
@@ -1758,10 +1755,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B68" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>6</v>
@@ -1775,7 +1772,7 @@
         <v>112</v>
       </c>
       <c r="B69" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>6</v>
@@ -1789,7 +1786,7 @@
         <v>113</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>6</v>
@@ -1803,7 +1800,7 @@
         <v>114</v>
       </c>
       <c r="B71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>6</v>
@@ -1817,7 +1814,7 @@
         <v>115</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>6</v>
@@ -1831,7 +1828,7 @@
         <v>116</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>6</v>
@@ -1845,7 +1842,7 @@
         <v>117</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>6</v>
@@ -1859,7 +1856,7 @@
         <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>6</v>
@@ -1873,7 +1870,7 @@
         <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>6</v>
@@ -1884,10 +1881,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B77" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>6</v>
@@ -1898,13 +1895,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>6</v>
@@ -1912,13 +1909,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" t="s">
         <v>124</v>
       </c>
-      <c r="B79" t="s">
-        <v>125</v>
-      </c>
       <c r="C79" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>6</v>
@@ -1929,7 +1926,7 @@
         <v>126</v>
       </c>
       <c r="B80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>6</v>
@@ -1943,7 +1940,7 @@
         <v>127</v>
       </c>
       <c r="B81" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>6</v>
@@ -1952,22 +1949,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>128</v>
-      </c>
-      <c r="B82" t="s">
-        <v>129</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D22" xr:uid="{4E015613-82F0-4B36-A479-6D699BFDFD98}"/>
+  <autoFilter ref="A1:D81" xr:uid="{4E015613-82F0-4B36-A479-6D699BFDFD98}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed file names to only be ASCII
</commit_message>
<xml_diff>
--- a/Book Documentation.xlsx
+++ b/Book Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinh\Desktop\College Stuff\Comp Ling Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E3C5DE-27B3-4425-A01A-144C9144261D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DA5658-DB5F-43B5-9144-CC37AD0710BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C94EF9E2-1198-47B8-9388-E321FADA7C2F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="130">
   <si>
     <t>Title</t>
   </si>
@@ -171,9 +171,6 @@
     <t xml:space="preserve">Victor Hugo </t>
   </si>
   <si>
-    <t>Les Misérables</t>
-  </si>
-  <si>
     <t>The Enchanted Wanderer</t>
   </si>
   <si>
@@ -414,13 +411,19 @@
     <t>The Magic Skin</t>
   </si>
   <si>
-    <t>Eugénie Grandet</t>
-  </si>
-  <si>
     <t>Le Grand Meaulnes</t>
   </si>
   <si>
     <t>Alain Fournier</t>
+  </si>
+  <si>
+    <t>Eugenie Grandet</t>
+  </si>
+  <si>
+    <t>Honore de Balzac</t>
+  </si>
+  <si>
+    <t>Les Miserables</t>
   </si>
 </sst>
 </file>
@@ -787,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE2798D-75E9-44CF-8467-CB97DDF729A5}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +817,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,7 +885,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1195,7 +1198,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
@@ -1209,10 +1212,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
         <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -1223,10 +1226,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
         <v>48</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -1237,7 +1240,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
         <v>16</v>
@@ -1251,7 +1254,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -1265,10 +1268,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
         <v>52</v>
-      </c>
-      <c r="B33" t="s">
-        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -1279,10 +1282,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
         <v>54</v>
-      </c>
-      <c r="B34" t="s">
-        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
@@ -1293,7 +1296,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
@@ -1307,7 +1310,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
         <v>21</v>
@@ -1321,7 +1324,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -1335,7 +1338,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -1349,7 +1352,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -1363,7 +1366,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
         <v>44</v>
@@ -1377,10 +1380,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
         <v>63</v>
-      </c>
-      <c r="B41" t="s">
-        <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
@@ -1391,10 +1394,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>6</v>
@@ -1405,10 +1408,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>6</v>
@@ -1419,10 +1422,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
         <v>68</v>
-      </c>
-      <c r="B44" t="s">
-        <v>69</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>6</v>
@@ -1433,10 +1436,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>6</v>
@@ -1447,10 +1450,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" t="s">
         <v>71</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>6</v>
@@ -1461,10 +1464,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
         <v>73</v>
-      </c>
-      <c r="B47" t="s">
-        <v>74</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
@@ -1475,10 +1478,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" t="s">
         <v>75</v>
-      </c>
-      <c r="B48" t="s">
-        <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>9</v>
@@ -1489,10 +1492,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
         <v>77</v>
-      </c>
-      <c r="B49" t="s">
-        <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>6</v>
@@ -1503,10 +1506,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" t="s">
         <v>79</v>
-      </c>
-      <c r="B50" t="s">
-        <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>6</v>
@@ -1517,10 +1520,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
         <v>81</v>
-      </c>
-      <c r="B51" t="s">
-        <v>82</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>6</v>
@@ -1531,10 +1534,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" t="s">
         <v>83</v>
-      </c>
-      <c r="B52" t="s">
-        <v>84</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>6</v>
@@ -1545,10 +1548,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>6</v>
@@ -1559,10 +1562,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>6</v>
@@ -1573,10 +1576,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" t="s">
         <v>87</v>
-      </c>
-      <c r="B55" t="s">
-        <v>88</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>6</v>
@@ -1587,10 +1590,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" t="s">
         <v>89</v>
-      </c>
-      <c r="B56" t="s">
-        <v>90</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
@@ -1601,10 +1604,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" t="s">
         <v>91</v>
-      </c>
-      <c r="B57" t="s">
-        <v>92</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>6</v>
@@ -1615,10 +1618,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" t="s">
         <v>93</v>
-      </c>
-      <c r="B58" t="s">
-        <v>94</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>6</v>
@@ -1629,10 +1632,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" t="s">
         <v>95</v>
-      </c>
-      <c r="B59" t="s">
-        <v>96</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>6</v>
@@ -1643,10 +1646,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>6</v>
@@ -1657,10 +1660,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" t="s">
         <v>98</v>
-      </c>
-      <c r="B61" t="s">
-        <v>99</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>6</v>
@@ -1671,10 +1674,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" t="s">
         <v>100</v>
-      </c>
-      <c r="B62" t="s">
-        <v>101</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>6</v>
@@ -1685,10 +1688,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" t="s">
         <v>102</v>
-      </c>
-      <c r="B63" t="s">
-        <v>103</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>6</v>
@@ -1699,10 +1702,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" t="s">
         <v>104</v>
-      </c>
-      <c r="B64" t="s">
-        <v>105</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>6</v>
@@ -1713,10 +1716,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" t="s">
         <v>106</v>
-      </c>
-      <c r="B65" t="s">
-        <v>107</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>6</v>
@@ -1727,10 +1730,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>6</v>
@@ -1741,10 +1744,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" t="s">
         <v>109</v>
-      </c>
-      <c r="B67" t="s">
-        <v>110</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>6</v>
@@ -1755,10 +1758,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>6</v>
@@ -1769,10 +1772,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>6</v>
@@ -1783,10 +1786,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>6</v>
@@ -1797,10 +1800,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>6</v>
@@ -1811,10 +1814,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>6</v>
@@ -1825,10 +1828,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>6</v>
@@ -1839,10 +1842,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>6</v>
@@ -1853,10 +1856,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>6</v>
@@ -1867,10 +1870,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" t="s">
         <v>119</v>
-      </c>
-      <c r="B76" t="s">
-        <v>120</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>6</v>
@@ -1881,10 +1884,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" t="s">
         <v>121</v>
-      </c>
-      <c r="B77" t="s">
-        <v>122</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>6</v>
@@ -1895,10 +1898,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" t="s">
         <v>123</v>
-      </c>
-      <c r="B78" t="s">
-        <v>124</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>9</v>
@@ -1909,10 +1912,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B79" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>6</v>
@@ -1923,10 +1926,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B80" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>6</v>
@@ -1937,10 +1940,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B81" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Recleaning the book data
</commit_message>
<xml_diff>
--- a/Book Documentation.xlsx
+++ b/Book Documentation.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trinh\Desktop\College Stuff\Comp Ling Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C0B9C6-7C4F-41AE-8684-CD5C62E5AA60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$81</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,331 +30,331 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="130">
   <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vietnamese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hungarian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authors Worth Looking Into</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Brothers Karamazov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fyodor Dostoevsky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alexandre Dumas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Three Musketeers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William Shakespeare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Eyre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charlotte Brontë</t>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Authors Worth Looking Into</t>
+  </si>
+  <si>
+    <t>The Brothers Karamazov</t>
+  </si>
+  <si>
+    <t>Fyodor Dostoevsky</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Alexandre Dumas</t>
+  </si>
+  <si>
+    <t>The Three Musketeers</t>
+  </si>
+  <si>
+    <t>William Shakespeare</t>
+  </si>
+  <si>
+    <t>Jane Eyre</t>
+  </si>
+  <si>
+    <t>Charlotte Brontë</t>
   </si>
   <si>
     <t xml:space="preserve">Victor Hugo </t>
   </si>
   <si>
-    <t xml:space="preserve">The Complete Short Stories of Ernest Hemingway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ernest Hemingway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Henryk Sienkiewicz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twenty Years After</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamlet</t>
+    <t>The Complete Short Stories of Ernest Hemingway</t>
+  </si>
+  <si>
+    <t>Ernest Hemingway</t>
+  </si>
+  <si>
+    <t>Henryk Sienkiewicz</t>
+  </si>
+  <si>
+    <t>Twenty Years After</t>
+  </si>
+  <si>
+    <t>Hamlet</t>
   </si>
   <si>
     <t xml:space="preserve">Scarlett </t>
   </si>
   <si>
-    <t xml:space="preserve">Alexandra Ripley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macbeth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Othello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resurrection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lev Tolstoy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crime and Punishment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burning Daylight</t>
+    <t>Alexandra Ripley</t>
+  </si>
+  <si>
+    <t>Macbeth</t>
+  </si>
+  <si>
+    <t>Othello</t>
+  </si>
+  <si>
+    <t>Resurrection</t>
+  </si>
+  <si>
+    <t>Lev Tolstoy</t>
+  </si>
+  <si>
+    <t>Crime and Punishment</t>
+  </si>
+  <si>
+    <t>Camille</t>
+  </si>
+  <si>
+    <t>Burning Daylight</t>
   </si>
   <si>
     <t xml:space="preserve">Jack London </t>
   </si>
   <si>
-    <t xml:space="preserve">Ten Years Later</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Taming of the Shrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Tales of Beedle the Bard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J. K. Rowling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Madonna in a Fur Coat</t>
+    <t>Ten Years Later</t>
+  </si>
+  <si>
+    <t>The Taming of the Shrew</t>
+  </si>
+  <si>
+    <t>The Tales of Beedle the Bard</t>
+  </si>
+  <si>
+    <t>J. K. Rowling</t>
+  </si>
+  <si>
+    <t>Madonna in a Fur Coat</t>
   </si>
   <si>
     <t xml:space="preserve">Sabahattin Ali </t>
   </si>
   <si>
-    <t xml:space="preserve">The Women's War</t>
+    <t>The Women's War</t>
   </si>
   <si>
     <t xml:space="preserve">Romeo and Juliet </t>
   </si>
   <si>
-    <t xml:space="preserve">Chicot the Jester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doctor Zhivago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boris Pasternak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Tempest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cymbeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wuthering Heights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emily Bronte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Farewell to Arms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Midsummer Night's Dream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Miserables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Enchanted Wanderer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nikolai Leskov</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quo Vadis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">King Lear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As You Like It</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gone with the Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Margaret Mitchell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peter the First</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aleksey Nikolaievich Tolstoy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anna Karenina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">War and Peace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Knight of Sainte-Hermine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Count of Monte Cristo</t>
+    <t>Chicot the Jester</t>
+  </si>
+  <si>
+    <t>Doctor Zhivago</t>
+  </si>
+  <si>
+    <t>Boris Pasternak</t>
+  </si>
+  <si>
+    <t>The Tempest</t>
+  </si>
+  <si>
+    <t>Cymbeline</t>
+  </si>
+  <si>
+    <t>Wuthering Heights</t>
+  </si>
+  <si>
+    <t>Emily Bronte</t>
+  </si>
+  <si>
+    <t>A Farewell to Arms</t>
+  </si>
+  <si>
+    <t>A Midsummer Night's Dream</t>
+  </si>
+  <si>
+    <t>Les Miserables</t>
+  </si>
+  <si>
+    <t>The Enchanted Wanderer</t>
+  </si>
+  <si>
+    <t>Nikolai Leskov</t>
+  </si>
+  <si>
+    <t>Quo Vadis</t>
+  </si>
+  <si>
+    <t>King Lear</t>
+  </si>
+  <si>
+    <t>As You Like It</t>
+  </si>
+  <si>
+    <t>Gone with the Wind</t>
+  </si>
+  <si>
+    <t>Margaret Mitchell</t>
+  </si>
+  <si>
+    <t>Peter the First</t>
+  </si>
+  <si>
+    <t>Aleksey Nikolaievich Tolstoy</t>
+  </si>
+  <si>
+    <t>Anna Karenina</t>
+  </si>
+  <si>
+    <t>War and Peace</t>
+  </si>
+  <si>
+    <t>The Knight of Sainte-Hermine</t>
+  </si>
+  <si>
+    <t>The Count of Monte Cristo</t>
   </si>
   <si>
     <t xml:space="preserve">The Black Tulip </t>
   </si>
   <si>
-    <t xml:space="preserve">Ninety-Three</t>
+    <t>Ninety-Three</t>
   </si>
   <si>
     <t xml:space="preserve">The Man Who Laughs </t>
   </si>
   <si>
-    <t xml:space="preserve">Victor Hugo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Desert and Wilderness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pride and Prejudice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Austen</t>
+    <t>Victor Hugo</t>
+  </si>
+  <si>
+    <t>In Desert and Wilderness</t>
+  </si>
+  <si>
+    <t>Pride and Prejudice</t>
+  </si>
+  <si>
+    <t>Jane Austen</t>
   </si>
   <si>
     <t xml:space="preserve">The Castle </t>
   </si>
   <si>
-    <t xml:space="preserve">Franz Kafka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Little Prince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antoine de Saint-Exupery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind, Sand and Stars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don Quixote</t>
+    <t>Franz Kafka</t>
+  </si>
+  <si>
+    <t>The Little Prince</t>
+  </si>
+  <si>
+    <t>Antoine de Saint-Exupery</t>
+  </si>
+  <si>
+    <t>Wind, Sand and Stars</t>
+  </si>
+  <si>
+    <t>Don Quixote</t>
   </si>
   <si>
     <t xml:space="preserve">Miguel de Cervantes </t>
   </si>
   <si>
-    <t xml:space="preserve">The Picture of Dorian Gray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oscar Wilde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Madame Bovary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gustave Flaubert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Candide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voltaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oliver Twist</t>
+    <t>The Picture of Dorian Gray</t>
+  </si>
+  <si>
+    <t>Oscar Wilde</t>
+  </si>
+  <si>
+    <t>Madame Bovary</t>
+  </si>
+  <si>
+    <t>Gustave Flaubert</t>
+  </si>
+  <si>
+    <t>Candide</t>
+  </si>
+  <si>
+    <t>Voltaire</t>
+  </si>
+  <si>
+    <t>Oliver Twist</t>
   </si>
   <si>
     <t xml:space="preserve">Charles Dickens </t>
   </si>
   <si>
-    <t xml:space="preserve">The Pickwick Papers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charles Dickens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great Expectations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Christmas Carol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Royal Game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stefan Zweig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Sorrows of Young Werther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Johann Wolfgang von Goethe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Diary Of a Young Girl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anne Frank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dubliners</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Joyce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ladies' Paradise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emile Zola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Therese Raquin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dracula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bram Stoker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iliad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Odyssey</t>
+    <t>The Pickwick Papers</t>
+  </si>
+  <si>
+    <t>Charles Dickens</t>
+  </si>
+  <si>
+    <t>Great Expectations</t>
+  </si>
+  <si>
+    <t>A Christmas Carol</t>
+  </si>
+  <si>
+    <t>The Royal Game</t>
+  </si>
+  <si>
+    <t>Stefan Zweig</t>
+  </si>
+  <si>
+    <t>The Sorrows of Young Werther</t>
+  </si>
+  <si>
+    <t>Johann Wolfgang von Goethe</t>
+  </si>
+  <si>
+    <t>The Diary Of a Young Girl</t>
+  </si>
+  <si>
+    <t>Anne Frank</t>
+  </si>
+  <si>
+    <t>Dubliners</t>
+  </si>
+  <si>
+    <t>James Joyce</t>
+  </si>
+  <si>
+    <t>The Ladies' Paradise</t>
+  </si>
+  <si>
+    <t>Emile Zola</t>
+  </si>
+  <si>
+    <t>Therese Raquin</t>
+  </si>
+  <si>
+    <t>Dracula</t>
+  </si>
+  <si>
+    <t>Bram Stoker</t>
+  </si>
+  <si>
+    <t>Iliad</t>
+  </si>
+  <si>
+    <t>Homer</t>
+  </si>
+  <si>
+    <t>Odyssey</t>
   </si>
   <si>
     <t xml:space="preserve">Homer </t>
   </si>
   <si>
-    <t xml:space="preserve">The Red and the Black</t>
+    <t>The Red and the Black</t>
   </si>
   <si>
     <t xml:space="preserve">Stendhal </t>
   </si>
   <si>
-    <t xml:space="preserve">The Barsac Mission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jules Verne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Waif of the Cynthia</t>
+    <t>The Barsac Mission</t>
+  </si>
+  <si>
+    <t>Jules Verne</t>
+  </si>
+  <si>
+    <t>The Waif of the Cynthia</t>
   </si>
   <si>
     <t xml:space="preserve">The Vanished Diamond </t>
@@ -358,92 +363,74 @@
     <t xml:space="preserve">Jules Verne </t>
   </si>
   <si>
-    <t xml:space="preserve">The Danube Pilot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Search of the Castaways</t>
+    <t>The Danube Pilot</t>
+  </si>
+  <si>
+    <t>In Search of the Castaways</t>
   </si>
   <si>
     <t xml:space="preserve">Around the World in Eighty Days </t>
   </si>
   <si>
-    <t xml:space="preserve">Five Weeks in a Balloon</t>
+    <t>Five Weeks in a Balloon</t>
   </si>
   <si>
     <t xml:space="preserve">The Mysterious Island </t>
   </si>
   <si>
-    <t xml:space="preserve">Dick Sand, A Captain at Fifteen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journey to the Center of the Earth</t>
+    <t>Dick Sand, A Captain at Fifteen</t>
+  </si>
+  <si>
+    <t>Journey to the Center of the Earth</t>
   </si>
   <si>
     <t xml:space="preserve">The Lighthouse at the End of the World </t>
   </si>
   <si>
-    <t xml:space="preserve">The Decameron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giovanni Boccaccio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Love</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivan Turgenev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Pere Goriot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Honoré de Balzac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Magic Skin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Honore de Balzac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eugenie Grandet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Grand Meaulnes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alain Fournier</t>
+    <t>The Decameron</t>
+  </si>
+  <si>
+    <t>Giovanni Boccaccio</t>
+  </si>
+  <si>
+    <t>First Love</t>
+  </si>
+  <si>
+    <t>Ivan Turgenev</t>
+  </si>
+  <si>
+    <t>Le Pere Goriot</t>
+  </si>
+  <si>
+    <t>Honoré de Balzac</t>
+  </si>
+  <si>
+    <t>The Magic Skin</t>
+  </si>
+  <si>
+    <t>Honore de Balzac</t>
+  </si>
+  <si>
+    <t>Eugenie Grandet</t>
+  </si>
+  <si>
+    <t>Le Grand Meaulnes</t>
+  </si>
+  <si>
+    <t>Alain Fournier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -461,7 +448,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -469,85 +456,348 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.29"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,15 +810,15 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -581,11 +831,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -598,11 +848,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -615,11 +865,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -632,11 +882,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -646,11 +896,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -660,11 +910,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -674,11 +924,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -688,11 +938,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -702,11 +952,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -716,11 +966,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -730,11 +980,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -744,11 +994,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -758,11 +1008,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -772,11 +1022,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -786,11 +1036,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -800,11 +1050,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -814,11 +1064,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -828,11 +1078,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -842,11 +1092,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -856,11 +1106,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -870,11 +1120,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -884,11 +1134,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -898,11 +1148,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -912,11 +1162,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -926,11 +1176,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -940,11 +1190,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -954,11 +1204,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -968,11 +1218,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -982,11 +1232,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -996,11 +1246,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1010,11 +1260,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>54</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1024,11 +1274,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>56</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1038,11 +1288,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1052,11 +1302,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1066,11 +1316,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1080,11 +1330,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1094,11 +1344,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1108,11 +1358,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1122,11 +1372,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1136,11 +1386,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1150,11 +1400,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>67</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1164,11 +1414,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" t="s">
         <v>69</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1178,11 +1428,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" t="s">
         <v>71</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1192,11 +1442,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" t="s">
         <v>71</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1206,25 +1456,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" t="s">
         <v>74</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" t="s">
         <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1234,11 +1484,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>77</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" t="s">
         <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -1248,11 +1498,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" t="s">
         <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -1262,11 +1512,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>81</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" t="s">
         <v>82</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -1276,11 +1526,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" t="s">
         <v>84</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1290,11 +1540,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" t="s">
         <v>82</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -1304,11 +1554,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" t="s">
         <v>82</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -1318,11 +1568,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>87</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" t="s">
         <v>88</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -1332,11 +1582,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" t="s">
         <v>90</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1346,11 +1596,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" t="s">
         <v>92</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -1360,11 +1610,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>93</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" t="s">
         <v>94</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -1374,11 +1624,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" t="s">
         <v>96</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -1388,11 +1638,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" t="s">
         <v>96</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -1402,11 +1652,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>98</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" t="s">
         <v>99</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -1416,11 +1666,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>100</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" t="s">
         <v>101</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -1430,11 +1680,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" t="s">
         <v>103</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -1444,11 +1694,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>104</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" t="s">
         <v>105</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -1458,11 +1708,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>106</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" t="s">
         <v>107</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -1472,11 +1722,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>108</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" t="s">
         <v>107</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -1486,11 +1736,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>109</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" t="s">
         <v>110</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -1500,11 +1750,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>111</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" t="s">
         <v>107</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -1514,11 +1764,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>112</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" t="s">
         <v>107</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -1528,11 +1778,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>113</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" t="s">
         <v>107</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -1542,11 +1792,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" t="s">
         <v>107</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -1556,11 +1806,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>115</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" t="s">
         <v>107</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -1570,11 +1820,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>116</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" t="s">
         <v>107</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -1584,11 +1834,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>117</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" t="s">
         <v>107</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -1598,11 +1848,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>118</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" t="s">
         <v>107</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -1612,11 +1862,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>119</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" t="s">
         <v>120</v>
       </c>
       <c r="C76" s="1" t="s">
@@ -1626,11 +1876,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>121</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" t="s">
         <v>122</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -1640,11 +1890,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>123</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" t="s">
         <v>124</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -1654,11 +1904,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>125</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" t="s">
         <v>126</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -1668,11 +1918,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>127</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" t="s">
         <v>126</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -1682,11 +1932,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>128</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" t="s">
         <v>129</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -1697,14 +1947,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D81"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:D81" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>